<commit_message>
SRS Login Register Modification
</commit_message>
<xml_diff>
--- a/Requirments/SRS.xlsx
+++ b/Requirments/SRS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ITI9M-Testing\Core\QA\WorkShop\Online-Mobile-Store-WebSite\Requirments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{032AE1E3-B110-4FF8-BB20-38F77404CAB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE6320BE-5372-408A-BBAA-F8628C63806A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="65">
   <si>
     <t>ID</t>
   </si>
@@ -124,36 +124,12 @@
     <t>SRS_Reg_019</t>
   </si>
   <si>
-    <t>SRS_Reg_020</t>
-  </si>
-  <si>
-    <t>SRS_Reg_021</t>
-  </si>
-  <si>
-    <t>SRS_Reg_022</t>
-  </si>
-  <si>
-    <t>SRS_Reg_023</t>
-  </si>
-  <si>
-    <t>SRS_Reg_024</t>
-  </si>
-  <si>
-    <t>SRS_Reg_025</t>
-  </si>
-  <si>
     <t>The username shall contain only alphabetic characters (a-z, A-Z).</t>
   </si>
   <si>
     <t>The username shall not contain spaces.</t>
   </si>
   <si>
-    <t>The username shall be unique; no other user shall have the same username.</t>
-  </si>
-  <si>
-    <t>If the username does not meet requirements Req_001,Reg_002,Reg_003, Reg_004 an error message "please enter valid data" shall be displayed.</t>
-  </si>
-  <si>
     <t>The email address shall adhere to a standard email format (e.g., [test12@gmail.com]).</t>
   </si>
   <si>
@@ -166,27 +142,15 @@
     <t>The password shall be hidden while typing.</t>
   </si>
   <si>
-    <t>If the email does not meet requirements Req_008,Reg_009,Reg_010 an error message "please enter valid data" shall be displayed.</t>
-  </si>
-  <si>
-    <t>If the password does not meet requirements Req_014,Reg_015,Reg_016,Reg_017 an error message "please enter valid data" shall be displayed.</t>
-  </si>
-  <si>
     <t>The confirm password shall match the password entered in Reg_014.</t>
   </si>
   <si>
-    <t>If the confirm password does not match the password, an error message "please enter valid data" shall be displayed.</t>
-  </si>
-  <si>
     <t>The address shall contain letters and numbers.</t>
   </si>
   <si>
     <t>The address shall not exceed 40 characters.</t>
   </si>
   <si>
-    <t>If the address does not meet requirements Req_026,Reg_027,Reg_028 an error message "please enter valid data" shall be displayed.</t>
-  </si>
-  <si>
     <t>The phone number shall contain only numbers.</t>
   </si>
   <si>
@@ -196,18 +160,12 @@
     <t>The system shall allow multiple accounts to be registered with the same phone number.</t>
   </si>
   <si>
-    <t>If the phone number does not meet requirements Req_032,Reg_033,Reg_034,Reg_035 an error message "please enter valid data" shall be displayed.</t>
-  </si>
-  <si>
     <t>The National ID shall contain only numbers.</t>
   </si>
   <si>
     <t>The National ID shall be exactly 14 digits long.</t>
   </si>
   <si>
-    <t>If the  does not meet requirements Req_032,Reg_033,Reg_034,Reg_035 an error message "please enter valid data" shall be displayed.</t>
-  </si>
-  <si>
     <t>Upon successful registration, the user shall be redirected to the Home Page.</t>
   </si>
   <si>
@@ -223,9 +181,6 @@
     <t>CRS_Login_003</t>
   </si>
   <si>
-    <t>The system shall check if the entered username and password match a valid user account</t>
-  </si>
-  <si>
     <t>If either the username or password is invalid, an error message "Please enter valid username or password" shall be displayed</t>
   </si>
   <si>
@@ -244,19 +199,22 @@
     <t>SRS_Login_005</t>
   </si>
   <si>
-    <t>SRS_Login_006</t>
-  </si>
-  <si>
-    <t>SRS_Login_007</t>
-  </si>
-  <si>
     <t>The user (Client &amp; Supplier) shall be able to enter a username and password.</t>
   </si>
   <si>
-    <t xml:space="preserve"> If the username and password are valid, the user (Client &amp; Supplier) shall be logged in successfully</t>
-  </si>
-  <si>
-    <t>SRS_Login_008</t>
+    <t>The username shall be unique not exit in database; no other user shall have the same username.</t>
+  </si>
+  <si>
+    <t>If all fields do not meet requirements above an error message "please enter valid data" shall be displayed.</t>
+  </si>
+  <si>
+    <t>The username shall be exit in database.</t>
+  </si>
+  <si>
+    <t>The password shall be associated to the username entered.</t>
+  </si>
+  <si>
+    <t>If the username and password are valid, the user (Client &amp; Supplier) shall be logged in successfully and go to HOME Page</t>
   </si>
 </sst>
 </file>
@@ -613,16 +571,16 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C231"/>
+  <dimension ref="A1:C222"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.88671875" customWidth="1"/>
-    <col min="2" max="2" width="141.21875" customWidth="1"/>
+    <col min="2" max="2" width="154.33203125" customWidth="1"/>
     <col min="3" max="3" width="23.88671875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -642,7 +600,7 @@
         <v>15</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>3</v>
@@ -653,7 +611,7 @@
         <v>16</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>4</v>
@@ -664,7 +622,7 @@
         <v>17</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>4</v>
@@ -675,7 +633,7 @@
         <v>18</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>5</v>
@@ -686,10 +644,10 @@
         <v>19</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.35">
@@ -697,10 +655,10 @@
         <v>20</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.35">
@@ -708,10 +666,10 @@
         <v>21</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.35">
@@ -719,43 +677,43 @@
         <v>22</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+      <c r="B10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+      <c r="B11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>13</v>
+      <c r="B12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -763,10 +721,10 @@
         <v>26</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -774,10 +732,10 @@
         <v>27</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -785,10 +743,10 @@
         <v>28</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -796,10 +754,10 @@
         <v>29</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -807,10 +765,10 @@
         <v>30</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -818,10 +776,10 @@
         <v>31</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -829,10 +787,10 @@
         <v>32</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -840,165 +798,111 @@
         <v>33</v>
       </c>
       <c r="B20" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B21" s="2" t="s">
+      <c r="B24" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="5" t="s">
-        <v>38</v>
-      </c>
       <c r="B25" s="2" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>66</v>
-      </c>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+    </row>
+    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+    </row>
+    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+    </row>
+    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+    </row>
+    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+    </row>
+    <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+    </row>
+    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+    </row>
+    <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+    </row>
+    <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
     </row>
     <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
@@ -1939,51 +1843,6 @@
       <c r="A222" s="1"/>
       <c r="B222" s="1"/>
       <c r="C222" s="1"/>
-    </row>
-    <row r="223" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A223" s="1"/>
-      <c r="B223" s="1"/>
-      <c r="C223" s="1"/>
-    </row>
-    <row r="224" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A224" s="1"/>
-      <c r="B224" s="1"/>
-      <c r="C224" s="1"/>
-    </row>
-    <row r="225" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A225" s="1"/>
-      <c r="B225" s="1"/>
-      <c r="C225" s="1"/>
-    </row>
-    <row r="226" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A226" s="1"/>
-      <c r="B226" s="1"/>
-      <c r="C226" s="1"/>
-    </row>
-    <row r="227" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A227" s="1"/>
-      <c r="B227" s="1"/>
-      <c r="C227" s="1"/>
-    </row>
-    <row r="228" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A228" s="1"/>
-      <c r="B228" s="1"/>
-      <c r="C228" s="1"/>
-    </row>
-    <row r="229" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A229" s="1"/>
-      <c r="B229" s="1"/>
-      <c r="C229" s="1"/>
-    </row>
-    <row r="230" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A230" s="1"/>
-      <c r="B230" s="1"/>
-      <c r="C230" s="1"/>
-    </row>
-    <row r="231" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A231" s="1"/>
-      <c r="B231" s="1"/>
-      <c r="C231" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
Doc: Added supplier requirements
</commit_message>
<xml_diff>
--- a/Requirments/SRS.xlsx
+++ b/Requirments/SRS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ITI9M-Testing\Core\QA\WorkShop\Online-Mobile-Store-WebSite\Requirments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Online-Mobile-Store-WebSite\Requirments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE6320BE-5372-408A-BBAA-F8628C63806A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F02B0609-ACF7-45BA-AF8A-FDCF572A2777}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="90">
   <si>
     <t>ID</t>
   </si>
@@ -215,6 +215,81 @@
   </si>
   <si>
     <t>If the username and password are valid, the user (Client &amp; Supplier) shall be logged in successfully and go to HOME Page</t>
+  </si>
+  <si>
+    <t>SRS_Supplier_001</t>
+  </si>
+  <si>
+    <t>CRS_Supplier_001</t>
+  </si>
+  <si>
+    <t>SRS_Supplier_002</t>
+  </si>
+  <si>
+    <t>SRS_Supplier_003</t>
+  </si>
+  <si>
+    <t>SRS_Supplier_004</t>
+  </si>
+  <si>
+    <t>SRS_Supplier_005</t>
+  </si>
+  <si>
+    <t>SRS_Supplier_006</t>
+  </si>
+  <si>
+    <t>SRS_Supplier_007</t>
+  </si>
+  <si>
+    <t>SRS_Supplier_008</t>
+  </si>
+  <si>
+    <t>SRS_Supplier_009</t>
+  </si>
+  <si>
+    <t>SRS_Supplier_010</t>
+  </si>
+  <si>
+    <t>CRS_Supplier_002</t>
+  </si>
+  <si>
+    <t>CRS_Supplier_003</t>
+  </si>
+  <si>
+    <t>CRS_Supplier_004</t>
+  </si>
+  <si>
+    <t>CRS_Supplier_006</t>
+  </si>
+  <si>
+    <t>Product ID : should following This Naming Conventional : [Brand/Category]_[ProductName]_[Size/Version]</t>
+  </si>
+  <si>
+    <t>Product Photo : should not exceed 300KB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product Price : should be Numeric Only and do not contain special </t>
+  </si>
+  <si>
+    <t>Product Price : should not contain special character like ($)</t>
+  </si>
+  <si>
+    <t>Product Platform : should choose IOS or Android</t>
+  </si>
+  <si>
+    <t>Product version : should be following this format [Major.Minor.Patch] like XXX.XXX.XXX</t>
+  </si>
+  <si>
+    <t>Supplier can ADD product with data (product id,product photo, product price, product version, product platform )</t>
+  </si>
+  <si>
+    <t>Supplier can UPDATE product by changing any of product data (product id,product photo, product price, product version, product platform) using Product ID</t>
+  </si>
+  <si>
+    <t>Supplier can DELETE product with Product ID</t>
+  </si>
+  <si>
+    <t>There is an Error message If the supplier enter Incorrect or Missing data "Invalid Data"</t>
   </si>
 </sst>
 </file>
@@ -573,18 +648,18 @@
   </sheetPr>
   <dimension ref="A1:C222"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A135" zoomScale="95" workbookViewId="0">
+      <selection activeCell="C150" sqref="C150:C159"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.88671875" customWidth="1"/>
-    <col min="2" max="2" width="154.33203125" customWidth="1"/>
-    <col min="3" max="3" width="23.88671875" customWidth="1"/>
+    <col min="1" max="1" width="23.90625" customWidth="1"/>
+    <col min="2" max="2" width="154.36328125" customWidth="1"/>
+    <col min="3" max="3" width="23.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" s="4" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -595,7 +670,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
         <v>15</v>
       </c>
@@ -606,7 +681,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A3" s="5" t="s">
         <v>16</v>
       </c>
@@ -617,7 +692,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A4" s="5" t="s">
         <v>17</v>
       </c>
@@ -628,7 +703,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A5" s="5" t="s">
         <v>18</v>
       </c>
@@ -639,7 +714,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A6" s="5" t="s">
         <v>19</v>
       </c>
@@ -650,7 +725,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A7" s="5" t="s">
         <v>20</v>
       </c>
@@ -661,7 +736,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A8" s="5" t="s">
         <v>21</v>
       </c>
@@ -672,7 +747,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A9" s="5" t="s">
         <v>22</v>
       </c>
@@ -683,7 +758,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="5" t="s">
         <v>23</v>
       </c>
@@ -694,7 +769,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="5" t="s">
         <v>24</v>
       </c>
@@ -705,7 +780,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="5" t="s">
         <v>25</v>
       </c>
@@ -716,7 +791,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="5" t="s">
         <v>26</v>
       </c>
@@ -727,7 +802,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="5" t="s">
         <v>27</v>
       </c>
@@ -738,7 +813,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="5" t="s">
         <v>28</v>
       </c>
@@ -749,7 +824,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="5" t="s">
         <v>29</v>
       </c>
@@ -760,7 +835,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="5" t="s">
         <v>30</v>
       </c>
@@ -771,7 +846,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="5" t="s">
         <v>31</v>
       </c>
@@ -782,7 +857,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="5" t="s">
         <v>32</v>
       </c>
@@ -793,7 +868,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="5" t="s">
         <v>33</v>
       </c>
@@ -804,7 +879,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="2" t="s">
         <v>54</v>
       </c>
@@ -815,7 +890,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="2" t="s">
         <v>55</v>
       </c>
@@ -826,7 +901,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="2" t="s">
         <v>56</v>
       </c>
@@ -837,7 +912,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="2" t="s">
         <v>57</v>
       </c>
@@ -848,7 +923,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="2" t="s">
         <v>58</v>
       </c>
@@ -859,987 +934,1047 @@
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
     </row>
-    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
     </row>
-    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
     </row>
-    <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
     </row>
-    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
     </row>
-    <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
     </row>
-    <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
     </row>
-    <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
     </row>
-    <row r="36" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
     </row>
-    <row r="37" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
     </row>
-    <row r="38" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
     </row>
-    <row r="39" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
     </row>
-    <row r="40" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
     </row>
-    <row r="41" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
     </row>
-    <row r="42" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
     </row>
-    <row r="43" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
     </row>
-    <row r="44" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
     </row>
-    <row r="45" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
     </row>
-    <row r="46" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
     </row>
-    <row r="47" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
     </row>
-    <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
     </row>
-    <row r="49" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
     </row>
-    <row r="50" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
     </row>
-    <row r="51" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
     </row>
-    <row r="52" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
     </row>
-    <row r="53" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
     </row>
-    <row r="54" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
     </row>
-    <row r="55" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
     </row>
-    <row r="56" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
     </row>
-    <row r="57" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
     </row>
-    <row r="58" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
     </row>
-    <row r="59" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
     </row>
-    <row r="60" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
     </row>
-    <row r="61" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
     </row>
-    <row r="62" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
     </row>
-    <row r="63" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
     </row>
-    <row r="64" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
     </row>
-    <row r="65" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
     </row>
-    <row r="66" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
     </row>
-    <row r="67" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
     </row>
-    <row r="68" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
     </row>
-    <row r="69" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
     </row>
-    <row r="70" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
     </row>
-    <row r="71" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
     </row>
-    <row r="72" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
     </row>
-    <row r="73" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
     </row>
-    <row r="74" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
     </row>
-    <row r="75" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
     </row>
-    <row r="76" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
     </row>
-    <row r="77" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
     </row>
-    <row r="78" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
     </row>
-    <row r="79" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
     </row>
-    <row r="80" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
     </row>
-    <row r="81" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
     </row>
-    <row r="82" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
     </row>
-    <row r="83" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
     </row>
-    <row r="84" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
     </row>
-    <row r="85" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
     </row>
-    <row r="86" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
     </row>
-    <row r="87" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
     </row>
-    <row r="88" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
     </row>
-    <row r="89" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
     </row>
-    <row r="90" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
     </row>
-    <row r="91" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
     </row>
-    <row r="92" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
     </row>
-    <row r="93" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
     </row>
-    <row r="94" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
     </row>
-    <row r="95" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
     </row>
-    <row r="96" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
     </row>
-    <row r="97" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
     </row>
-    <row r="98" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
     </row>
-    <row r="99" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
     </row>
-    <row r="100" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
     </row>
-    <row r="101" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
     </row>
-    <row r="102" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
     </row>
-    <row r="103" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
     </row>
-    <row r="104" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
     </row>
-    <row r="105" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
     </row>
-    <row r="106" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
     </row>
-    <row r="107" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
     </row>
-    <row r="108" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
     </row>
-    <row r="109" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
     </row>
-    <row r="110" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
     </row>
-    <row r="111" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
     </row>
-    <row r="112" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
     </row>
-    <row r="113" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
     </row>
-    <row r="114" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
     </row>
-    <row r="115" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
     </row>
-    <row r="116" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
     </row>
-    <row r="117" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
     </row>
-    <row r="118" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
     </row>
-    <row r="119" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
     </row>
-    <row r="120" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
     </row>
-    <row r="121" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
     </row>
-    <row r="122" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
     </row>
-    <row r="123" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A123" s="1"/>
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
     </row>
-    <row r="124" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
     </row>
-    <row r="125" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
     </row>
-    <row r="126" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
     </row>
-    <row r="127" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
     </row>
-    <row r="128" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
     </row>
-    <row r="129" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A129" s="1"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
     </row>
-    <row r="130" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A130" s="1"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
     </row>
-    <row r="131" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
     </row>
-    <row r="132" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A132" s="1"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
     </row>
-    <row r="133" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
     </row>
-    <row r="134" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A134" s="1"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
     </row>
-    <row r="135" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
     </row>
-    <row r="136" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
     </row>
-    <row r="137" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A137" s="1"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
     </row>
-    <row r="138" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A138" s="1"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
     </row>
-    <row r="139" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A139" s="1"/>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
     </row>
-    <row r="140" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
     </row>
-    <row r="141" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A141" s="1"/>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
     </row>
-    <row r="142" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A142" s="1"/>
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
     </row>
-    <row r="143" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A143" s="1"/>
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
     </row>
-    <row r="144" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A144" s="1"/>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
     </row>
-    <row r="145" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A145" s="1"/>
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
     </row>
-    <row r="146" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A146" s="1"/>
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
     </row>
-    <row r="147" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A147" s="1"/>
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
     </row>
-    <row r="148" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A148" s="1"/>
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
     </row>
-    <row r="149" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A149" s="1"/>
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
     </row>
-    <row r="150" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A150" s="1"/>
-      <c r="B150" s="1"/>
-      <c r="C150" s="1"/>
-    </row>
-    <row r="151" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A151" s="1"/>
-      <c r="B151" s="1"/>
-      <c r="C151" s="1"/>
-    </row>
-    <row r="152" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A152" s="1"/>
-      <c r="B152" s="1"/>
-      <c r="C152" s="1"/>
-    </row>
-    <row r="153" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A153" s="1"/>
-      <c r="B153" s="1"/>
-      <c r="C153" s="1"/>
-    </row>
-    <row r="154" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A154" s="1"/>
-      <c r="B154" s="1"/>
-      <c r="C154" s="1"/>
-    </row>
-    <row r="155" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A155" s="1"/>
-      <c r="B155" s="1"/>
-      <c r="C155" s="1"/>
-    </row>
-    <row r="156" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A156" s="1"/>
-      <c r="B156" s="1"/>
-      <c r="C156" s="1"/>
-    </row>
-    <row r="157" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A157" s="1"/>
-      <c r="B157" s="1"/>
-      <c r="C157" s="1"/>
-    </row>
-    <row r="158" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A158" s="1"/>
-      <c r="B158" s="1"/>
-      <c r="C158" s="1"/>
-    </row>
-    <row r="159" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A159" s="1"/>
-      <c r="B159" s="1"/>
-      <c r="C159" s="1"/>
-    </row>
-    <row r="160" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A150" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A151" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A152" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A153" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A154" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A155" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A156" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A157" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A158" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A159" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A160" s="1"/>
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
     </row>
-    <row r="161" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A161" s="1"/>
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
     </row>
-    <row r="162" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A162" s="1"/>
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
     </row>
-    <row r="163" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A163" s="1"/>
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
     </row>
-    <row r="164" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A164" s="1"/>
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
     </row>
-    <row r="165" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A165" s="1"/>
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
     </row>
-    <row r="166" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A166" s="1"/>
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
     </row>
-    <row r="167" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A167" s="1"/>
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
     </row>
-    <row r="168" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A168" s="1"/>
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
     </row>
-    <row r="169" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A169" s="1"/>
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
     </row>
-    <row r="170" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A170" s="1"/>
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
     </row>
-    <row r="171" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A171" s="1"/>
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
     </row>
-    <row r="172" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A172" s="1"/>
       <c r="B172" s="1"/>
       <c r="C172" s="1"/>
     </row>
-    <row r="173" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A173" s="1"/>
       <c r="B173" s="1"/>
       <c r="C173" s="1"/>
     </row>
-    <row r="174" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A174" s="1"/>
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
     </row>
-    <row r="175" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A175" s="1"/>
       <c r="B175" s="1"/>
       <c r="C175" s="1"/>
     </row>
-    <row r="176" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A176" s="1"/>
       <c r="B176" s="1"/>
       <c r="C176" s="1"/>
     </row>
-    <row r="177" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A177" s="1"/>
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
     </row>
-    <row r="178" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A178" s="1"/>
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
     </row>
-    <row r="179" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A179" s="1"/>
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
     </row>
-    <row r="180" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A180" s="1"/>
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
     </row>
-    <row r="181" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A181" s="1"/>
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
     </row>
-    <row r="182" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A182" s="1"/>
       <c r="B182" s="1"/>
       <c r="C182" s="1"/>
     </row>
-    <row r="183" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A183" s="1"/>
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
     </row>
-    <row r="184" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A184" s="1"/>
       <c r="B184" s="1"/>
       <c r="C184" s="1"/>
     </row>
-    <row r="185" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A185" s="1"/>
       <c r="B185" s="1"/>
       <c r="C185" s="1"/>
     </row>
-    <row r="186" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A186" s="1"/>
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
     </row>
-    <row r="187" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A187" s="1"/>
       <c r="B187" s="1"/>
       <c r="C187" s="1"/>
     </row>
-    <row r="188" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A188" s="1"/>
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
     </row>
-    <row r="189" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A189" s="1"/>
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
     </row>
-    <row r="190" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A190" s="1"/>
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
     </row>
-    <row r="191" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A191" s="1"/>
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
     </row>
-    <row r="192" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A192" s="1"/>
       <c r="B192" s="1"/>
       <c r="C192" s="1"/>
     </row>
-    <row r="193" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A193" s="1"/>
       <c r="B193" s="1"/>
       <c r="C193" s="1"/>
     </row>
-    <row r="194" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A194" s="1"/>
       <c r="B194" s="1"/>
       <c r="C194" s="1"/>
     </row>
-    <row r="195" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A195" s="1"/>
       <c r="B195" s="1"/>
       <c r="C195" s="1"/>
     </row>
-    <row r="196" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A196" s="1"/>
       <c r="B196" s="1"/>
       <c r="C196" s="1"/>
     </row>
-    <row r="197" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A197" s="1"/>
       <c r="B197" s="1"/>
       <c r="C197" s="1"/>
     </row>
-    <row r="198" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A198" s="1"/>
       <c r="B198" s="1"/>
       <c r="C198" s="1"/>
     </row>
-    <row r="199" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A199" s="1"/>
       <c r="B199" s="1"/>
       <c r="C199" s="1"/>
     </row>
-    <row r="200" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A200" s="1"/>
       <c r="B200" s="1"/>
       <c r="C200" s="1"/>
     </row>
-    <row r="201" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A201" s="1"/>
       <c r="B201" s="1"/>
       <c r="C201" s="1"/>
     </row>
-    <row r="202" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A202" s="1"/>
       <c r="B202" s="1"/>
       <c r="C202" s="1"/>
     </row>
-    <row r="203" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A203" s="1"/>
       <c r="B203" s="1"/>
       <c r="C203" s="1"/>
     </row>
-    <row r="204" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A204" s="1"/>
       <c r="B204" s="1"/>
       <c r="C204" s="1"/>
     </row>
-    <row r="205" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A205" s="1"/>
       <c r="B205" s="1"/>
       <c r="C205" s="1"/>
     </row>
-    <row r="206" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A206" s="1"/>
       <c r="B206" s="1"/>
       <c r="C206" s="1"/>
     </row>
-    <row r="207" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A207" s="1"/>
       <c r="B207" s="1"/>
       <c r="C207" s="1"/>
     </row>
-    <row r="208" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A208" s="1"/>
       <c r="B208" s="1"/>
       <c r="C208" s="1"/>
     </row>
-    <row r="209" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A209" s="1"/>
       <c r="B209" s="1"/>
       <c r="C209" s="1"/>
     </row>
-    <row r="210" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A210" s="1"/>
       <c r="B210" s="1"/>
       <c r="C210" s="1"/>
     </row>
-    <row r="211" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A211" s="1"/>
       <c r="B211" s="1"/>
       <c r="C211" s="1"/>
     </row>
-    <row r="212" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A212" s="1"/>
       <c r="B212" s="1"/>
       <c r="C212" s="1"/>
     </row>
-    <row r="213" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A213" s="1"/>
       <c r="B213" s="1"/>
       <c r="C213" s="1"/>
     </row>
-    <row r="214" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A214" s="1"/>
       <c r="B214" s="1"/>
       <c r="C214" s="1"/>
     </row>
-    <row r="215" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A215" s="1"/>
       <c r="B215" s="1"/>
       <c r="C215" s="1"/>
     </row>
-    <row r="216" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A216" s="1"/>
       <c r="B216" s="1"/>
       <c r="C216" s="1"/>
     </row>
-    <row r="217" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A217" s="1"/>
       <c r="B217" s="1"/>
       <c r="C217" s="1"/>
     </row>
-    <row r="218" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A218" s="1"/>
       <c r="B218" s="1"/>
       <c r="C218" s="1"/>
     </row>
-    <row r="219" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A219" s="1"/>
       <c r="B219" s="1"/>
       <c r="C219" s="1"/>
     </row>
-    <row r="220" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A220" s="1"/>
       <c r="B220" s="1"/>
       <c r="C220" s="1"/>
     </row>
-    <row r="221" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A221" s="1"/>
       <c r="B221" s="1"/>
       <c r="C221" s="1"/>
     </row>
-    <row r="222" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A222" s="1"/>
       <c r="B222" s="1"/>
       <c r="C222" s="1"/>

</xml_diff>

<commit_message>
Doc: updated SRS file according to comments in review file
</commit_message>
<xml_diff>
--- a/Requirments/SRS.xlsx
+++ b/Requirments/SRS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\QA\Online-Mobile-Store-WebSite\Requirments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{002C2A31-0943-424B-AE92-A9C0FE6DB37D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{425B6FA9-72E5-4773-BAB2-FA4E7E86C5AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="130">
   <si>
     <t>ID</t>
   </si>
@@ -328,9 +328,6 @@
     <t>SRS_Client_005</t>
   </si>
   <si>
-    <t>The client shall be able to view  the contents of their cart. This includes product names, quantities, prices, and the ability to increment, decrement product count, or remove items.</t>
-  </si>
-  <si>
     <t>CRS_client_006</t>
   </si>
   <si>
@@ -364,9 +361,6 @@
     <t>CRS_client_008</t>
   </si>
   <si>
-    <t>SRS_Client_010</t>
-  </si>
-  <si>
     <t>After placing an order, a confirmation message "Your order is placed successfully" should appear, and the client should be redirected to the history of buys</t>
   </si>
   <si>
@@ -394,7 +388,28 @@
     <t>SRS_Client_013</t>
   </si>
   <si>
-    <t>if the produc becomes out of stock an message appears behind the produc "out of stock"</t>
+    <t>SRS_Client_014</t>
+  </si>
+  <si>
+    <t>CRS_Client_003</t>
+  </si>
+  <si>
+    <t>When the client tries to select a product that is out of stock an message should appear "product is out of stock"</t>
+  </si>
+  <si>
+    <t>if the product becomes out of stock an message appears the product "out of stock"</t>
+  </si>
+  <si>
+    <t>The client shall be able to view  the contents of their cart. This includes product names, quantities, prices.</t>
+  </si>
+  <si>
+    <t>the client should be able to increment, decrement product count, or remove items.</t>
+  </si>
+  <si>
+    <t>SRS_Client_0010</t>
+  </si>
+  <si>
+    <t>SRS_Client_015</t>
   </si>
 </sst>
 </file>
@@ -758,10 +773,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C111"/>
+  <dimension ref="A1:C113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="113" zoomScaleNormal="113" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="113" zoomScaleNormal="113" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1084,10 +1099,10 @@
         <v>98</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1098,125 +1113,125 @@
         <v>99</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>102</v>
+        <v>124</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>100</v>
+        <v>119</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>114</v>
+        <v>128</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>109</v>
+        <v>125</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>112</v>
+        <v>116</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>108</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>86</v>
+        <v>122</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>111</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>66</v>
+        <v>109</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>67</v>
+        <v>129</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>80</v>
+        <v>113</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>78</v>
+        <v>112</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>66</v>
@@ -1224,21 +1239,21 @@
     </row>
     <row r="42" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>66</v>
@@ -1246,10 +1261,10 @@
     </row>
     <row r="44" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>66</v>
@@ -1257,10 +1272,10 @@
     </row>
     <row r="45" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>66</v>
@@ -1268,46 +1283,58 @@
     </row>
     <row r="46" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B50" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C50" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="1"/>
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-    </row>
-    <row r="50" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="1"/>
-      <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
     </row>
     <row r="51" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
@@ -1613,6 +1640,16 @@
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
+    </row>
+    <row r="112" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="1"/>
+      <c r="B112" s="1"/>
+      <c r="C112" s="1"/>
+    </row>
+    <row r="113" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="1"/>
+      <c r="B113" s="1"/>
+      <c r="C113" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>